<commit_message>
Updates to sample metadata
</commit_message>
<xml_diff>
--- a/data/sample_sheets/G000304_Broomfield.sample_metadata.xlsx
+++ b/data/sample_sheets/G000304_Broomfield.sample_metadata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26212"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EF03884-8CCE-48D8-A741-10B2B5AB5160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45544DDD-8C6D-42FE-AD73-1D2412C49A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Tube</t>
   </si>
@@ -48,7 +48,22 @@
     <t>Progressed to scRNA-seq</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>removed_1</t>
+  </si>
+  <si>
+    <t>removed_2</t>
+  </si>
+  <si>
+    <t>removed_3</t>
+  </si>
+  <si>
+    <t>removed_4</t>
+  </si>
+  <si>
+    <t>removed_5</t>
+  </si>
+  <si>
+    <t>removed_6</t>
   </si>
   <si>
     <t>Cell line</t>
@@ -461,7 +476,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -686,7 +701,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -754,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -771,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -788,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -839,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -941,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>

</xml_diff>